<commit_message>
contact us V 0.22.0
</commit_message>
<xml_diff>
--- a/org.trimatek.digideal/releases.xlsx
+++ b/org.trimatek.digideal/releases.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
@@ -18,10 +18,53 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>versión</t>
+  </si>
+  <si>
+    <t>fecha despliegue</t>
+  </si>
+  <si>
+    <t>fecha prueba</t>
+  </si>
+  <si>
+    <t>novedades</t>
+  </si>
+  <si>
+    <t>resultado</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>características prueba</t>
+  </si>
+  <si>
+    <t>0.21.0</t>
+  </si>
+  <si>
+    <t>3 contratos en simultáneo</t>
+  </si>
+  <si>
+    <t>0.22.0</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -49,8 +92,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -331,12 +376,172 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="45.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1">
+        <v>43380</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1">
+        <v>43380</v>
+      </c>
+      <c r="D3" s="1"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C10" s="1"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="1"/>
+      <c r="D11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+    </row>
+    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+    </row>
+    <row r="23" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+    </row>
+    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C30" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>